<commit_message>
added a few stats (and changed TODOs)
</commit_message>
<xml_diff>
--- a/rbdc/doc/data/statistics.xlsx
+++ b/rbdc/doc/data/statistics.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pgemind/Documents/private/projects/rbdc/doc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{39EED286-365F-CC4A-A5B2-D69BCBADDF75}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2B4EBC30-DE30-BB4F-9F47-8350D3EAC523}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15540" yWindow="2940" windowWidth="16640" windowHeight="15080" activeTab="3" xr2:uid="{1DD5BE52-7325-724C-BEF1-591DD18DFDBE}"/>
+    <workbookView xWindow="12180" yWindow="780" windowWidth="16640" windowHeight="15080" xr2:uid="{1DD5BE52-7325-724C-BEF1-591DD18DFDBE}"/>
   </bookViews>
   <sheets>
-    <sheet name="weapons" sheetId="1" r:id="rId1"/>
-    <sheet name="armors" sheetId="2" r:id="rId2"/>
-    <sheet name="offhands" sheetId="3" r:id="rId3"/>
-    <sheet name="trinkets" sheetId="4" r:id="rId4"/>
-    <sheet name="valuables" sheetId="5" r:id="rId5"/>
+    <sheet name="Statistics" sheetId="6" r:id="rId1"/>
+    <sheet name="weapons" sheetId="1" r:id="rId2"/>
+    <sheet name="armors" sheetId="2" r:id="rId3"/>
+    <sheet name="offhands" sheetId="3" r:id="rId4"/>
+    <sheet name="trinkets" sheetId="4" r:id="rId5"/>
+    <sheet name="valuables" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
   <si>
     <t>value</t>
   </si>
@@ -98,6 +99,39 @@
   </si>
   <si>
     <t>bomb</t>
+  </si>
+  <si>
+    <t>Key figure</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>avg. Dmg</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>weapons</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>armors</t>
+  </si>
+  <si>
+    <t>offhands</t>
+  </si>
+  <si>
+    <t>trinkets</t>
+  </si>
+  <si>
+    <t>valuables</t>
+  </si>
+  <si>
+    <t>avg. Value</t>
   </si>
 </sst>
 </file>
@@ -141,9 +175,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -457,16 +493,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071AD21D-4C91-6745-A2FA-94874D50E56A}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2">
+        <f ca="1">AVERAGE(INDIRECT(B2&amp;"!H:H"))</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:C6" ca="1" si="0">AVERAGE(INDIRECT(B3&amp;"!H:H"))</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.6666666666666665</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2">
+        <f ca="1">AVERAGE(INDIRECT(B6&amp;"!C:C"))</f>
+        <v>5.333333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:C10" ca="1" si="1">AVERAGE(INDIRECT(B7&amp;"!C:C"))</f>
+        <v>27.666666666666668</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10BC9B9-46F9-3943-B041-3D9DC0F1CDC2}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -488,8 +641,11 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -511,8 +667,12 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <f>SUM(D2:G2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -534,8 +694,12 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="0">SUM(D3:G3)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -557,112 +721,9 @@
       <c r="G4">
         <v>0</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C68809-6F9C-0E44-A22A-3CA0FFDBC5AD}">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="H4">
+        <f t="shared" si="0"/>
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3">
-        <v>50</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>15</v>
-      </c>
-      <c r="F3">
-        <v>30</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>20</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -671,16 +732,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF68C554-4A6D-7343-876B-6F8E3A390700}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C68809-6F9C-0E44-A22A-3CA0FFDBC5AD}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -702,51 +763,89 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>SUM(D2:G2)</f>
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="0">SUM(D3:G3)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -755,16 +854,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD398B59-89F2-2B43-9346-A6C966FF998B}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF68C554-4A6D-7343-876B-6F8E3A390700}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -786,42 +885,49 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>SUM(D2:G2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -830,7 +936,17 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="0">SUM(D3:G3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -839,16 +955,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E181464-3DFC-2A4D-83DD-1F53138B43EC}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD398B59-89F2-2B43-9346-A6C966FF998B}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -870,8 +986,97 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f>SUM(D2:G2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="0">SUM(D3:G3)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E181464-3DFC-2A4D-83DD-1F53138B43EC}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -880,18 +1085,6 @@
       </c>
       <c r="C2">
         <v>10</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>